<commit_message>
done almost all revisions and sections/ only left minip 14 pivottable and charts
</commit_message>
<xml_diff>
--- a/section8Revision/revision.xlsx
+++ b/section8Revision/revision.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomas\Pulpit\excelLearning\section8Revision\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6B45B19-7E69-4371-A61C-F60ECDE14058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B996934-BB22-456F-9AE0-FAD25386CBC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,8 +36,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="149">
   <si>
     <t>🔡 FUNKCJE TEKSTOWE I ICH PUŁAPKI</t>
   </si>
@@ -1275,6 +1298,1134 @@
   </si>
   <si>
     <t xml:space="preserve">nie wiem </t>
+  </si>
+  <si>
+    <t>🔡 FUNKCJE TEKSTOWE (1–10)</t>
+  </si>
+  <si>
+    <t>1. Jak wyodrębnić nazwisko z pełnego imienia i nazwiska typu: „Anna Maria Kowalska”, gdy nazwisko zawsze ostatnie?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2. Co zrobi </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>=TEXTJOIN("-", TRUE, A1:C1)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> i czym się różni od </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>CONCAT()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">3. Jak usunąć znaki specjalne (np. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>@</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>#</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) z tekstu bez Power Query?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">4. Co zwróci </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>=LEFT("INV/2024-08",FIND("/",A1)-1)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>?</t>
+    </r>
+  </si>
+  <si>
+    <t>5. Jak wyodrębnić NIP z tekstu „Faktura: PL1234567890 – wystawiona 2024-01-01”?</t>
+  </si>
+  <si>
+    <t>6. Jak rozbić numer konta bankowego na bloki po 4 cyfry?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">7. Jak działa </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>TEXTSPLIT()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> z wieloma delimiterami i co się stanie, gdy delimitery się nachodzą?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">8. Co robi </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>=MID(A1,SEARCH(":",A1)+2,5)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>? Dla tekstu „Kod: 98765 – zamknięte”.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">9. Jak za pomocą </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>REPLACE()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> wyczyścić drugą i trzecią literę z ciągu tekstowego?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">10. Czym różni się </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>TEXTJOIN(",",TRUE,A1:A5)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> od </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>TEXTJOIN(",",FALSE,A1:A5)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>?</t>
+    </r>
+  </si>
+  <si>
+    <t>TEXTSPLIT("Anna Maria Kowalska";" ";)</t>
+  </si>
+  <si>
+    <t>rozni się tym ze możliwe jest dodanie delimetra oraz tym ze może pominac puste pola, fukncja wyzej polaczy wyrazy z trzech komorek a miedzy kazda komorka wstawi -</t>
+  </si>
+  <si>
+    <t>metoda regex replace</t>
+  </si>
+  <si>
+    <t>zwroci date faktury</t>
+  </si>
+  <si>
+    <t>Faktura: PL1234567890 – wystawiona 2024-01-01</t>
+  </si>
+  <si>
+    <t>find -</t>
+  </si>
+  <si>
+    <t>findSpace</t>
+  </si>
+  <si>
+    <t>faktura</t>
+  </si>
+  <si>
+    <t>no dopasowuje delimter po kolei z tego nawiasu w ciele formuly do delimitera napotkanego w texcie. Gdy się delimtery nachodza to funkcja nie zadziala</t>
+  </si>
+  <si>
+    <t>zwraca kod 98765</t>
+  </si>
+  <si>
+    <t>REPLACE("ABCDEF", 2, 2, "")</t>
+  </si>
+  <si>
+    <t>tym ze z TRUE pomija puste komorki a z false nie</t>
+  </si>
+  <si>
+    <t>🧠 LOGIKA I WARUNKI (11–20)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">11. Jak za pomocą </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>IFS()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> zakodować: „&lt;100 zł – niski, 100–1000 – średni, &gt;1000 – wysoki”?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">12. Co zwróci </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>=IF("0",1,0)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> i dlaczego?</t>
+    </r>
+  </si>
+  <si>
+    <t>13. Jak napisać formułę: „jeśli A1 zawiera tekst 'test', to 'OK', inaczej 'NOK'”?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">14. Czym różni się </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>OR(A1&gt;5,A1&lt;0)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> od </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>A1&gt;5 OR A1&lt;0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">15. Kiedy </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>NOT()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> jest przydatny w połączeniu z </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>ISBLANK()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">16. Jak za pomocą </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>LET()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> uprościć warunek oparty o wielokrotne </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>LEN(TRIM(A1))</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>?</t>
+    </r>
+  </si>
+  <si>
+    <t>17. Jak zbudować warunek: „jeśli A1 jest tekstem lub puste, to daj 0, inaczej wartość A1”?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">18. Co zwraca </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>=N(TRUE)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> i do czego można to wykorzystać?</t>
+    </r>
+  </si>
+  <si>
+    <t>19. Jak zbudować formułę zwracającą „BRAK”, jeśli A1 jest błędem lub pustą komórką?</t>
+  </si>
+  <si>
+    <t>20. Jak porównać dwie kolumny i zwrócić „match” tylko wtedy, gdy zawartość i typ są takie same?</t>
+  </si>
+  <si>
+    <t>ifs(a1&lt;100;"niski";and(a1&gt;100;a1&lt;1000);"sredni";a1&gt;1000;"Wysoki")</t>
+  </si>
+  <si>
+    <t>zwroci value! Bo nie ma jakby no warunku funkcji if</t>
+  </si>
+  <si>
+    <t>if(a1="test";"ok";"nok")</t>
+  </si>
+  <si>
+    <t>tym ze drugie wyrazenie  to blad?</t>
+  </si>
+  <si>
+    <t>kiedy chcemy sprawdzic jako TRUE czy komorka nie jest pusta</t>
+  </si>
+  <si>
+    <t>nie wiem wytlumacz mi</t>
+  </si>
+  <si>
+    <t>żeby zliczyc ilosc wartosci true w kolumnie?</t>
+  </si>
+  <si>
+    <t>if(or(istext(a1);islbank(a1));0;A1</t>
+  </si>
+  <si>
+    <t>iferror(or(iserror(a1);isblank(a1);"Brak";</t>
+  </si>
+  <si>
+    <t>if(a1=a2;match(a1;a2);"not match")</t>
+  </si>
+  <si>
+    <t>🔍 WYSZUKIWANIE I DOPASOWANIA (21–30)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">21. Jak za pomocą </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>XLOOKUP()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> znaleźć ostatnią niepustą wartość w kolumnie?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">22. Co zwróci </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>=XMATCH(5,{1,3,5,5,7},0,-1)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> i czym różni się od </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>MATCH()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">23. Jak działa </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>LOOKUP(2,1/(A1:A100&lt;&gt;""),A1:A100)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>?</t>
+    </r>
+  </si>
+  <si>
+    <t>24. Jak dopasować klienta z największą sprzedażą – bez sortowania danych?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">25. Czym różni się </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>INDEX(MATCH(...))</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> od </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>XLOOKUP(...)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, jeśli dane są wielokolumnowe?</t>
+    </r>
+  </si>
+  <si>
+    <t>26. Jak zbudować elastyczny lookup po 2 warunkach (np. ID klienta i region)?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">27. Co zwróci </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>=XLOOKUP(9999, A1:A10, B1:B10, "Brak", -1)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> jeśli dane nie są posortowane?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">28. Jak dynamicznie wybrać kolumnę do zwrotu w </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>INDEX()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>?</t>
+    </r>
+  </si>
+  <si>
+    <t>29. Jak zbudować formułę, która wyciągnie pierwszą wartość spełniającą warunek z zakresu?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">30. Jak działa </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>FILTER()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>INDEX()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>COUNTA()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> w wyciąganiu </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ostatniej pasującej</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> wartości?</t>
+    </r>
+  </si>
+  <si>
+    <t>📆 DATY I CZAS (31–35)</t>
+  </si>
+  <si>
+    <t>31. Jak przeliczyć datę na numer kwartału?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">32. Czym różni się </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>WORKDAY()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> od </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>NETWORKDAYS()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>?</t>
+    </r>
+  </si>
+  <si>
+    <t>33. Jak obliczyć datę końca miesiąca 3 miesiące od dziś?</t>
+  </si>
+  <si>
+    <t>34. Jak sformatować datę tak, by zawsze pokazywała „1. dzień miesiąca”?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">35. Jak policzyć pełne lata i miesiące między dwoma datami – bez </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>DATEDIF()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>?</t>
+    </r>
+  </si>
+  <si>
+    <t>❌ BŁĘDY, TYPY, KONTROLA (36–40)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">36. Co zwróci </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>=TYPE("123")</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> i czym się różni od </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>ISNUMBER("123")</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">37. Jakie są najczęstsze powody #VALUE! w zagnieżdżonych </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>TEXT()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> i </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>IF()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">38. Jak zabezpieczyć </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>XLOOKUP()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> przed błędami typu </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>#N/A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> i </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>#REF!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – bez </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>IFERROR()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">39. Jakie typy błędów rozpoznaje </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>ERROR.TYPE()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> i co zwraca dla #NAME!?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">40. Kiedy użyć </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>T()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> i </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>N()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> w analizie danych? Daj 2 praktyczne zastosowania.</t>
+    </r>
+  </si>
+  <si>
+    <t>xlookup(True;row&lt;&gt;"";row;0;-1)</t>
+  </si>
+  <si>
+    <t>zwroci pozycje pierwszego znalezionego 5 od konca</t>
+  </si>
+  <si>
+    <t>XLOOKUP(MAX(B2:B10), B2:B10, A2:A10)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no co zwroci odpowiadajaca wartosc jeśli się znajdzie 9999 w a1:a10 a jeśli nie to pierwsza mniejsza </t>
+  </si>
+  <si>
+    <t>ROUNDUP(MONTH(A2)/3,0)</t>
+  </si>
+  <si>
+    <t>workday zwraca date miedzy dwoma dniami, a networkdays liczbe tygodni miedzy nimi</t>
+  </si>
+  <si>
+    <t>datevalue przekonwertowac obie obliczyc nastpenie zrobic year z tych obliczen</t>
+  </si>
+  <si>
+    <t>eomonth(date-1)+1 nw dlaczego tak</t>
+  </si>
+  <si>
+    <t>nw</t>
+  </si>
+  <si>
+    <t>type zwraca integer odpowiadajac typowi danej a isnumber zwraca truefalse</t>
+  </si>
+  <si>
+    <t>hmmmm np. brak seperatoru</t>
+  </si>
+  <si>
+    <t>no napisac w ciele formuly co zrobic gdy jest error, xlookup to umozliwia</t>
+  </si>
+  <si>
+    <t>wszystkie typy, dla name zwraca 5</t>
+  </si>
+  <si>
+    <t>żeby sprawdzic czy kolumna zawiera jednorodny typ danych a drugie nw</t>
   </si>
 </sst>
 </file>
@@ -1621,8 +2772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="I17" activeCellId="1" sqref="A1:E118 I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2074,5 +3225,523 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{084D951D-1532-4212-BA9B-CFD60E21A358}">
+  <dimension ref="A1:D102"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="I66" sqref="I66"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="18">
+      <c r="A1" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="2"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="2" t="str" cm="1">
+        <f t="array" ref="A4:C4">_xlfn.TEXTSPLIT("Anna Maria Kowalska"," ",)</f>
+        <v>Anna</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Maria</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Kowalska</v>
+      </c>
+      <c r="D4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="2"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>84</v>
+      </c>
+      <c r="C14" t="s">
+        <v>85</v>
+      </c>
+      <c r="D14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15">
+        <f>LEN(A13)</f>
+        <v>45</v>
+      </c>
+      <c r="B15">
+        <f>FIND(" –",A13)</f>
+        <v>22</v>
+      </c>
+      <c r="C15">
+        <f>FIND(" ",A13)</f>
+        <v>9</v>
+      </c>
+      <c r="D15" t="str">
+        <f>MID(A13,C15+1,B15-C15)</f>
+        <v xml:space="preserve">PL1234567890 </v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" ht="18">
+      <c r="A30" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" s="2"/>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="2" t="e">
+        <f>IF("0",1,0)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="B35" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" ht="18">
+      <c r="A53" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" s="2"/>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" ht="18">
+      <c r="A77" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" s="2"/>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="18">
+      <c r="A91" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="A92" s="2"/>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94" s="2">
+        <f>TYPE("123")</f>
+        <v>2</v>
+      </c>
+      <c r="B94" t="b">
+        <f>ISNUMBER("123")</f>
+        <v>0</v>
+      </c>
+      <c r="D94" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="A95" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="A96" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1">
+      <c r="A97" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1">
+      <c r="A100" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1">
+      <c r="A101" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1">
+      <c r="A102" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>